<commit_message>
leger changement pour etre raccord avec taiga
</commit_message>
<xml_diff>
--- a/Documentation/Repartition_fonctionnalité_par_sprint_et_équipe.xlsx
+++ b/Documentation/Repartition_fonctionnalité_par_sprint_et_équipe.xlsx
@@ -840,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,7 +933,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>30</v>

</xml_diff>